<commit_message>
update ERA tables with correct fisheries
</commit_message>
<xml_diff>
--- a/output/2023/ERA/table1.xlsx
+++ b/output/2023/ERA/table1.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -393,7 +393,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Räkfiske med rist i Skagerrak, Kattegatt och Nordsjön</t>
+          <t>Räkfiske rist;  3a4</t>
         </is>
       </c>
     </row>
@@ -404,14 +404,14 @@
         </is>
       </c>
       <c r="B3">
-        <v>90.3</v>
+        <v>90.09999999999999</v>
       </c>
       <c r="C3">
-        <v>90.3</v>
+        <v>90.09999999999999</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Räkfiske med rist/tunnel i Skagerrak, Kattegatt och Nordsjön</t>
+          <t>Räkfiske tunnel och rist;  3a4</t>
         </is>
       </c>
     </row>
@@ -425,11 +425,11 @@
         <v>3.4</v>
       </c>
       <c r="C4">
-        <v>93.7</v>
+        <v>93.5</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Räkfiske med rist/tunnel i Skagerrak, Kattegatt och Nordsjön</t>
+          <t>Räkfiske tunnel och rist;  3a4</t>
         </is>
       </c>
     </row>
@@ -443,11 +443,11 @@
         <v>2.8</v>
       </c>
       <c r="C5">
-        <v>96.5</v>
+        <v>96.3</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Räkfiske med rist/tunnel i Skagerrak, Kattegatt och Nordsjön</t>
+          <t>Räkfiske tunnel och rist;  3a4</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Fiske med kräftburar</t>
+          <t>Fiske med kräftburar;  3a</t>
         </is>
       </c>
     </row>
@@ -476,14 +476,14 @@
         </is>
       </c>
       <c r="B7">
-        <v>46.4</v>
+        <v>44.4</v>
       </c>
       <c r="C7">
-        <v>46.4</v>
+        <v>44.4</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Fiske med passiva redskap i Skagerrak och Kattegatt</t>
+          <t>Fiske med passiva redskap;  3a</t>
         </is>
       </c>
     </row>
@@ -494,14 +494,14 @@
         </is>
       </c>
       <c r="B8">
-        <v>18.4</v>
+        <v>17.7</v>
       </c>
       <c r="C8">
-        <v>64.8</v>
+        <v>62.1</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Fiske med passiva redskap i Skagerrak och Kattegatt</t>
+          <t>Fiske med passiva redskap;  3a</t>
         </is>
       </c>
     </row>
@@ -512,14 +512,14 @@
         </is>
       </c>
       <c r="B9">
-        <v>14.6</v>
+        <v>14</v>
       </c>
       <c r="C9">
-        <v>79.40000000000001</v>
+        <v>76.09999999999999</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Fiske med passiva redskap i Skagerrak och Kattegatt</t>
+          <t>Fiske med passiva redskap;  3a</t>
         </is>
       </c>
     </row>
@@ -530,500 +530,500 @@
         </is>
       </c>
       <c r="B10">
-        <v>6.6</v>
+        <v>6.3</v>
       </c>
       <c r="C10">
-        <v>86</v>
+        <v>82.40000000000001</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Fiske med passiva redskap i Skagerrak och Kattegatt</t>
+          <t>Fiske med passiva redskap;  3a</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Tretömmad skärlånga</t>
+          <t>Skärsnultra</t>
         </is>
       </c>
       <c r="B11">
         <v>3.3</v>
       </c>
       <c r="C11">
-        <v>89.3</v>
+        <v>85.7</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Fiske med passiva redskap i Skagerrak och Kattegatt</t>
+          <t>Fiske med passiva redskap;  3a</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Torsk</t>
+          <t>Stensnultra</t>
         </is>
       </c>
       <c r="B12">
-        <v>2.1</v>
+        <v>3.1</v>
       </c>
       <c r="C12">
-        <v>91.40000000000001</v>
+        <v>88.8</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Fiske med passiva redskap i Skagerrak och Kattegatt</t>
+          <t>Fiske med passiva redskap;  3a</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Äkta tunga</t>
+          <t>Torsk</t>
         </is>
       </c>
       <c r="B13">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="C13">
-        <v>92.8</v>
+        <v>90.8</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Fiske med passiva redskap i Skagerrak och Kattegatt</t>
+          <t>Fiske med passiva redskap;  3a</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Sill/Strömming</t>
+          <t>Äkta tunga</t>
         </is>
       </c>
       <c r="B14">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="C14">
-        <v>94.2</v>
+        <v>92.2</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Fiske med passiva redskap i Skagerrak och Kattegatt</t>
+          <t>Fiske med passiva redskap;  3a</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Piggvar</t>
+          <t>Sill / strömming</t>
         </is>
       </c>
       <c r="B15">
-        <v>1.1</v>
+        <v>1.3</v>
       </c>
       <c r="C15">
-        <v>95.2</v>
+        <v>93.5</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Fiske med passiva redskap i Skagerrak och Kattegatt</t>
+          <t>Fiske med passiva redskap;  3a</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Havskräfta</t>
+          <t>Piggvar</t>
         </is>
       </c>
       <c r="B16">
-        <v>93.59999999999999</v>
+        <v>1</v>
       </c>
       <c r="C16">
-        <v>93.59999999999999</v>
+        <v>94.5</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter kräfta och fisk i Kattegatt</t>
+          <t>Fiske med passiva redskap;  3a</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Fjärsing</t>
+          <t>Bleka / lyrtorsk</t>
         </is>
       </c>
       <c r="B17">
-        <v>1.9</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <v>95.5</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter kräfta och fisk i Kattegatt</t>
+          <t>Fiske med passiva redskap;  3a</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Torsk</t>
+          <t>Havskräfta</t>
         </is>
       </c>
       <c r="B18">
-        <v>29</v>
+        <v>93.59999999999999</v>
       </c>
       <c r="C18">
-        <v>29</v>
+        <v>93.59999999999999</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter fisk i Skagerrak</t>
+          <t>Bottentrål havskräfta och fisk;  3a21</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Kolja</t>
+          <t>Fjärsing</t>
         </is>
       </c>
       <c r="B19">
-        <v>17.7</v>
+        <v>1.9</v>
       </c>
       <c r="C19">
-        <v>46.7</v>
+        <v>95.5</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter fisk i Skagerrak</t>
+          <t>Bottentrål havskräfta och fisk;  3a21</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Rödtunga</t>
+          <t>Torsk</t>
         </is>
       </c>
       <c r="B20">
-        <v>10.1</v>
+        <v>29</v>
       </c>
       <c r="C20">
-        <v>56.8</v>
+        <v>29</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter fisk i Skagerrak</t>
+          <t>Bottentrål fisk;  3a20</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Havskräfta</t>
+          <t>Kolja</t>
         </is>
       </c>
       <c r="B21">
-        <v>9.699999999999999</v>
+        <v>17.7</v>
       </c>
       <c r="C21">
-        <v>66.5</v>
+        <v>46.7</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter fisk i Skagerrak</t>
+          <t>Bottentrål fisk;  3a20</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Gråsej</t>
+          <t>Rödtunga</t>
         </is>
       </c>
       <c r="B22">
-        <v>9.300000000000001</v>
+        <v>10</v>
       </c>
       <c r="C22">
-        <v>75.8</v>
+        <v>56.8</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter fisk i Skagerrak</t>
+          <t>Bottentrål fisk;  3a20</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Marulk</t>
+          <t>Havskräfta</t>
         </is>
       </c>
       <c r="B23">
-        <v>7.3</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="C23">
-        <v>83.09999999999999</v>
+        <v>66.40000000000001</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter fisk i Skagerrak</t>
+          <t>Bottentrål fisk;  3a20</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Kummel</t>
+          <t>Gråsej</t>
         </is>
       </c>
       <c r="B24">
-        <v>5.7</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="C24">
-        <v>88.8</v>
+        <v>75.7</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter fisk i Skagerrak</t>
+          <t>Bottentrål fisk;  3a20</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Rödspotta</t>
+          <t>Marulk</t>
         </is>
       </c>
       <c r="B25">
-        <v>5.3</v>
+        <v>7.3</v>
       </c>
       <c r="C25">
-        <v>94.2</v>
+        <v>83.09999999999999</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter fisk i Skagerrak</t>
+          <t>Bottentrål fisk;  3a20</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Bleka</t>
+          <t>Kummel</t>
         </is>
       </c>
       <c r="B26">
-        <v>1.2</v>
+        <v>5.7</v>
       </c>
       <c r="C26">
-        <v>95.40000000000001</v>
+        <v>88.8</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter fisk i Skagerrak</t>
+          <t>Bottentrål fisk;  3a20</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Havskräfta</t>
+          <t>Rödspätta</t>
         </is>
       </c>
       <c r="B27">
-        <v>79.3</v>
+        <v>5.3</v>
       </c>
       <c r="C27">
-        <v>79.3</v>
+        <v>94.09999999999999</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter kräfta och fisk i Skagerrak</t>
+          <t>Bottentrål fisk;  3a20</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Torsk</t>
+          <t>Bleka / lyrtorsk</t>
         </is>
       </c>
       <c r="B28">
-        <v>6.9</v>
+        <v>1.2</v>
       </c>
       <c r="C28">
-        <v>86.3</v>
+        <v>95.3</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter kräfta och fisk i Skagerrak</t>
+          <t>Bottentrål fisk;  3a20</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Marulk</t>
+          <t>Havskräfta</t>
         </is>
       </c>
       <c r="B29">
-        <v>2.7</v>
+        <v>79.3</v>
       </c>
       <c r="C29">
-        <v>88.90000000000001</v>
+        <v>79.3</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter kräfta och fisk i Skagerrak</t>
+          <t>Bottentrål havskräfta och fisk;  3a20</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Rödtunga</t>
+          <t>Torsk</t>
         </is>
       </c>
       <c r="B30">
-        <v>2.5</v>
+        <v>6.9</v>
       </c>
       <c r="C30">
-        <v>91.40000000000001</v>
+        <v>86.2</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter kräfta och fisk i Skagerrak</t>
+          <t>Bottentrål havskräfta och fisk;  3a20</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Kolja</t>
+          <t>Marulk</t>
         </is>
       </c>
       <c r="B31">
-        <v>1.5</v>
+        <v>2.7</v>
       </c>
       <c r="C31">
-        <v>93</v>
+        <v>88.90000000000001</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter kräfta och fisk i Skagerrak</t>
+          <t>Bottentrål havskräfta och fisk;  3a20</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Gråsej</t>
+          <t>Rödtunga</t>
         </is>
       </c>
       <c r="B32">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="C32">
-        <v>94.40000000000001</v>
+        <v>91.40000000000001</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter kräfta och fisk i Skagerrak</t>
+          <t>Bottentrål havskräfta och fisk;  3a20</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Rödspotta</t>
+          <t>Kolja</t>
         </is>
       </c>
       <c r="B33">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="C33">
-        <v>95.7</v>
+        <v>92.90000000000001</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter kräfta och fisk i Skagerrak</t>
+          <t>Bottentrål havskräfta och fisk;  3a20</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Havskräfta</t>
+          <t>Gråsej</t>
         </is>
       </c>
       <c r="B34">
-        <v>98.59999999999999</v>
+        <v>1.5</v>
       </c>
       <c r="C34">
-        <v>98.59999999999999</v>
+        <v>94.40000000000001</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter kräfta med rist i Skagerrak och Kattegatt</t>
+          <t>Bottentrål havskräfta och fisk;  3a20</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Torsk</t>
+          <t>Rödspätta</t>
         </is>
       </c>
       <c r="B35">
-        <v>41.8</v>
+        <v>1.2</v>
       </c>
       <c r="C35">
-        <v>41.8</v>
+        <v>95.59999999999999</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Fiske i Öresund</t>
+          <t>Bottentrål havskräfta och fisk;  3a20</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Sill/Strömming</t>
+          <t>Havskräfta</t>
         </is>
       </c>
       <c r="B36">
-        <v>23.7</v>
+        <v>98.59999999999999</v>
       </c>
       <c r="C36">
-        <v>65.5</v>
+        <v>98.59999999999999</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Fiske i Öresund</t>
+          <t>Bottentrål havskräfta rist;  3a</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Ål</t>
+          <t>Torsk</t>
         </is>
       </c>
       <c r="B37">
-        <v>11.8</v>
+        <v>68</v>
       </c>
       <c r="C37">
-        <v>77.3</v>
+        <v>68</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Fiske i Öresund</t>
+          <t>Passiva redskap (torsk); 22-24</t>
         </is>
       </c>
     </row>
@@ -1034,572 +1034,770 @@
         </is>
       </c>
       <c r="B38">
-        <v>8.9</v>
+        <v>14.9</v>
       </c>
       <c r="C38">
-        <v>86.2</v>
+        <v>82.90000000000001</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Fiske i Öresund</t>
+          <t>Passiva redskap (torsk); 22-24</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Rödspotta</t>
+          <t>Rödspätta</t>
         </is>
       </c>
       <c r="B39">
-        <v>3.8</v>
+        <v>6.5</v>
       </c>
       <c r="C39">
-        <v>90</v>
+        <v>89.40000000000001</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Fiske i Öresund</t>
+          <t>Passiva redskap (torsk); 22-24</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Makrill</t>
+          <t>Äkta tunga</t>
         </is>
       </c>
       <c r="B40">
-        <v>3.1</v>
+        <v>3.3</v>
       </c>
       <c r="C40">
-        <v>93.09999999999999</v>
+        <v>92.7</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Fiske i Öresund</t>
+          <t>Passiva redskap (torsk); 22-24</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Äkta tunga</t>
+          <t>Skrubbskädda</t>
         </is>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>2.2</v>
       </c>
       <c r="C41">
-        <v>95.09999999999999</v>
+        <v>94.90000000000001</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Fiske i Öresund</t>
+          <t>Passiva redskap (torsk); 22-24</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Torsk</t>
+          <t>Slätvar</t>
         </is>
       </c>
       <c r="B42">
-        <v>93</v>
+        <v>2</v>
       </c>
       <c r="C42">
-        <v>93</v>
+        <v>96.90000000000001</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter torsk i Östersjön</t>
+          <t>Passiva redskap (torsk); 22-24</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Skrubbskädda</t>
+          <t>Ål</t>
         </is>
       </c>
       <c r="B43">
-        <v>3.9</v>
+        <v>20.8</v>
       </c>
       <c r="C43">
-        <v>96.90000000000001</v>
+        <v>20.8</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter torsk i Östersjön</t>
+          <t>Fiske med övriga passiva redskap; 22-32</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Ål</t>
+          <t>Sill / strömming</t>
         </is>
       </c>
       <c r="B44">
-        <v>52.1</v>
+        <v>19.9</v>
       </c>
       <c r="C44">
-        <v>52.1</v>
+        <v>40.7</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Fiske med passiva redskap i centrala och södra Östersjön</t>
+          <t>Fiske med övriga passiva redskap; 22-32</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Abborre</t>
+          <t>Lax</t>
         </is>
       </c>
       <c r="B45">
-        <v>14.3</v>
+        <v>18.7</v>
       </c>
       <c r="C45">
-        <v>66.40000000000001</v>
+        <v>59.4</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Fiske med passiva redskap i centrala och södra Östersjön</t>
+          <t>Fiske med övriga passiva redskap; 22-32</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Piggvar</t>
+          <t>Siklöja</t>
         </is>
       </c>
       <c r="B46">
-        <v>7.3</v>
+        <v>14.1</v>
       </c>
       <c r="C46">
-        <v>73.8</v>
+        <v>73.5</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Fiske med passiva redskap i centrala och södra Östersjön</t>
+          <t>Fiske med övriga passiva redskap; 22-32</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Skrubbskädda</t>
+          <t>Sikar</t>
         </is>
       </c>
       <c r="B47">
-        <v>7.3</v>
+        <v>10.9</v>
       </c>
       <c r="C47">
-        <v>81.09999999999999</v>
+        <v>84.40000000000001</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Fiske med passiva redskap i centrala och södra Östersjön</t>
+          <t>Fiske med övriga passiva redskap; 22-32</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Torsk</t>
+          <t>Abborre</t>
         </is>
       </c>
       <c r="B48">
-        <v>6.6</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="C48">
-        <v>87.7</v>
+        <v>93.59999999999999</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Fiske med passiva redskap i centrala och södra Östersjön</t>
+          <t>Fiske med övriga passiva redskap; 22-32</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Sill/Strömming</t>
+          <t>Torsk</t>
         </is>
       </c>
       <c r="B49">
-        <v>5.1</v>
+        <v>1.6</v>
       </c>
       <c r="C49">
-        <v>92.8</v>
+        <v>95.3</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Fiske med passiva redskap i centrala och södra Östersjön</t>
+          <t>Fiske med övriga passiva redskap; 22-32</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Gädda</t>
+          <t>Torsk</t>
         </is>
       </c>
       <c r="B50">
-        <v>2.2</v>
+        <v>92.90000000000001</v>
       </c>
       <c r="C50">
-        <v>95</v>
+        <v>92.90000000000001</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Fiske med passiva redskap i centrala och södra Östersjön</t>
+          <t>Fiske med stormaskig bottentrål (torsk); 25-32</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Gös</t>
+          <t>Skrubbskädda</t>
         </is>
       </c>
       <c r="B51">
-        <v>1.9</v>
+        <v>5.7</v>
       </c>
       <c r="C51">
-        <v>96.90000000000001</v>
+        <v>98.59999999999999</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Fiske med passiva redskap i centrala och södra Östersjön</t>
+          <t>Fiske med stormaskig bottentrål (torsk); 25-32</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Siklöja</t>
+          <t>Skrubbskädda</t>
         </is>
       </c>
       <c r="B52">
-        <v>39.5</v>
+        <v>31.6</v>
       </c>
       <c r="C52">
-        <v>39.5</v>
+        <v>31.6</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Fiske med passiva redskap i norra Östersjön</t>
+          <t>Passiva redskap (torsk); 25-32</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Sill/Strömming</t>
+          <t>Piggvar</t>
         </is>
       </c>
       <c r="B53">
-        <v>39.1</v>
+        <v>23.6</v>
       </c>
       <c r="C53">
-        <v>78.59999999999999</v>
+        <v>55.2</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Fiske med passiva redskap i norra Östersjön</t>
+          <t>Passiva redskap (torsk); 25-32</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Abborre</t>
+          <t>Torsk</t>
         </is>
       </c>
       <c r="B54">
-        <v>18.3</v>
+        <v>16.5</v>
       </c>
       <c r="C54">
-        <v>96.90000000000001</v>
+        <v>71.7</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Fiske med passiva redskap i norra Östersjön</t>
+          <t>Passiva redskap (torsk); 25-32</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Siklöja</t>
+          <t>Abborre</t>
         </is>
       </c>
       <c r="B55">
-        <v>99.09999999999999</v>
+        <v>15.7</v>
       </c>
       <c r="C55">
-        <v>99.09999999999999</v>
+        <v>87.40000000000001</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Fiske efter siklöja med bottentrål</t>
+          <t>Passiva redskap (torsk); 25-32</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Sill/Strömming</t>
+          <t>Gädda</t>
         </is>
       </c>
       <c r="B56">
-        <v>55.7</v>
+        <v>6.5</v>
       </c>
       <c r="C56">
-        <v>55.7</v>
+        <v>93.90000000000001</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Pelagiskt fiske med aktiva redskap</t>
+          <t>Passiva redskap (torsk); 25-32</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Skarpsill</t>
+          <t>Sikar</t>
         </is>
       </c>
       <c r="B57">
-        <v>29.2</v>
+        <v>2.6</v>
       </c>
       <c r="C57">
-        <v>84.90000000000001</v>
+        <v>96.40000000000001</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Pelagiskt fiske med aktiva redskap</t>
+          <t>Passiva redskap (torsk); 25-32</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Tobis</t>
+          <t>Siklöja</t>
         </is>
       </c>
       <c r="B58">
-        <v>10.2</v>
+        <v>97.2</v>
       </c>
       <c r="C58">
-        <v>95.09999999999999</v>
+        <v>97.2</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Pelagiskt fiske med aktiva redskap</t>
+          <t>Fiske med finmaskig bottentrål efter pelagiska arter; 30-31</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Torsk</t>
+          <t>Sill / strömming</t>
         </is>
       </c>
       <c r="B59">
-        <v>32.7</v>
+        <v>84.3</v>
       </c>
       <c r="C59">
-        <v>32.7</v>
+        <v>84.3</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter fisk i Nordsjön</t>
+          <t>Pelagiskt fiske med aktiva redskap (flyttrål, vad); 21-24</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Gråsej</t>
+          <t>Skarpsill</t>
         </is>
       </c>
       <c r="B60">
-        <v>30</v>
+        <v>14.2</v>
       </c>
       <c r="C60">
-        <v>62.6</v>
+        <v>98.5</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter fisk i Nordsjön</t>
+          <t>Pelagiskt fiske med aktiva redskap (flyttrål, vad); 21-24</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Marulk</t>
+          <t>Torsk</t>
         </is>
       </c>
       <c r="B61">
-        <v>13.4</v>
+        <v>32.7</v>
       </c>
       <c r="C61">
-        <v>76</v>
+        <v>32.7</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter fisk i Nordsjön</t>
+          <t>Bottentrål fisk;  4</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Bleka</t>
+          <t>Gråsej</t>
         </is>
       </c>
       <c r="B62">
-        <v>5.9</v>
+        <v>30</v>
       </c>
       <c r="C62">
-        <v>81.90000000000001</v>
+        <v>62.6</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter fisk i Nordsjön</t>
+          <t>Bottentrål fisk;  4</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Kolja</t>
+          <t>Marulk</t>
         </is>
       </c>
       <c r="B63">
-        <v>4.9</v>
+        <v>13.4</v>
       </c>
       <c r="C63">
-        <v>86.8</v>
+        <v>76</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter fisk i Nordsjön</t>
+          <t>Bottentrål fisk;  4</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Kummel</t>
+          <t>Bleka / lyrtorsk</t>
         </is>
       </c>
       <c r="B64">
-        <v>2.8</v>
+        <v>5.9</v>
       </c>
       <c r="C64">
-        <v>89.59999999999999</v>
+        <v>81.90000000000001</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter fisk i Nordsjön</t>
+          <t>Bottentrål fisk;  4</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Långa</t>
+          <t>Kolja</t>
         </is>
       </c>
       <c r="B65">
-        <v>2.4</v>
+        <v>4.9</v>
       </c>
       <c r="C65">
-        <v>92</v>
+        <v>86.8</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter fisk i Nordsjön</t>
+          <t>Bottentrål fisk;  4</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Hälleflundra</t>
+          <t>Kummel</t>
         </is>
       </c>
       <c r="B66">
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
       <c r="C66">
-        <v>93.8</v>
+        <v>89.59999999999999</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter fisk i Nordsjön</t>
+          <t>Bottentrål fisk;  4</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Havskatt</t>
+          <t>Långa</t>
         </is>
       </c>
       <c r="B67">
-        <v>1.7</v>
+        <v>2.4</v>
       </c>
       <c r="C67">
-        <v>95.5</v>
+        <v>92</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Bottentrålfiske efter fisk i Nordsjön</t>
+          <t>Bottentrål fisk;  4</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Lax</t>
+          <t>Hälleflundra</t>
         </is>
       </c>
       <c r="B68">
-        <v>89.2</v>
+        <v>1.8</v>
       </c>
       <c r="C68">
-        <v>89.2</v>
+        <v>93.8</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Fiske efter lax</t>
+          <t>Bottentrål fisk;  4</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Siklöja</t>
+          <t>Havskatter</t>
         </is>
       </c>
       <c r="B69">
-        <v>7.4</v>
+        <v>1.7</v>
       </c>
       <c r="C69">
-        <v>96.59999999999999</v>
+        <v>95.5</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Fiske efter lax</t>
+          <t>Bottentrål fisk;  4</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Torsk</t>
+        </is>
+      </c>
+      <c r="B70">
+        <v>93.2</v>
+      </c>
+      <c r="C70">
+        <v>93.2</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Fiske med stormaskig bottentrål (torsk); 22-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Rödspätta</t>
+        </is>
+      </c>
+      <c r="B71">
+        <v>3.6</v>
+      </c>
+      <c r="C71">
+        <v>96.8</v>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Fiske med stormaskig bottentrål (torsk); 22-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Skarpsill</t>
+        </is>
+      </c>
+      <c r="B72">
+        <v>58.1</v>
+      </c>
+      <c r="C72">
+        <v>58.1</v>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Pelagiskt fiske med aktiva redskap (flyttrål, vad); 25-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Sill / strömming</t>
+        </is>
+      </c>
+      <c r="B73">
+        <v>41.4</v>
+      </c>
+      <c r="C73">
+        <v>99.59999999999999</v>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Pelagiskt fiske med aktiva redskap (flyttrål, vad); 25-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Sill / strömming</t>
+        </is>
+      </c>
+      <c r="B74">
+        <v>70.8</v>
+      </c>
+      <c r="C74">
+        <v>70.8</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Pelagiskt fiske med aktiva redskap (flyttrål, vad); 3a4</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Skarpsill</t>
+        </is>
+      </c>
+      <c r="B75">
+        <v>14.5</v>
+      </c>
+      <c r="C75">
+        <v>85.3</v>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Pelagiskt fiske med aktiva redskap (flyttrål, vad); 3a4</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Makrill</t>
+        </is>
+      </c>
+      <c r="B76">
+        <v>9.800000000000001</v>
+      </c>
+      <c r="C76">
+        <v>95.09999999999999</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Pelagiskt fiske med aktiva redskap (flyttrål, vad); 3a4</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Sill / strömming</t>
+        </is>
+      </c>
+      <c r="B77">
+        <v>98.09999999999999</v>
+      </c>
+      <c r="C77">
+        <v>98.09999999999999</v>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Pelagiskt fiske med aktiva redskap (flyttrål, vad); 30-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Tobisfiskar</t>
+        </is>
+      </c>
+      <c r="B78">
+        <v>99.59999999999999</v>
+      </c>
+      <c r="C78">
+        <v>99.59999999999999</v>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Pelagiskt fiske med aktiva redskap (bottentrål);  3a204</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Sill / strömming</t>
+        </is>
+      </c>
+      <c r="B79">
+        <v>60.2</v>
+      </c>
+      <c r="C79">
+        <v>60.2</v>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Fiske med finmaskig bottentrål efter pelagiska arter; 25-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Skarpsill</t>
+        </is>
+      </c>
+      <c r="B80">
+        <v>39.3</v>
+      </c>
+      <c r="C80">
+        <v>99.40000000000001</v>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Fiske med finmaskig bottentrål efter pelagiska arter; 25-29</t>
         </is>
       </c>
     </row>

</xml_diff>